<commit_message>
Remove old Colab notebook and add mock databases
</commit_message>
<xml_diff>
--- a/input/personal_data_change.xlsx
+++ b/input/personal_data_change.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/g/Documents/Data_change_portfolio/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/g/Documents/pdf_form_filler/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89D24C2-45A8-8741-AD32-8C20F7277F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CD0A94-556A-F342-B654-0115A8797D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -562,7 +562,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,11 +574,13 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -590,13 +592,21 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -662,16 +672,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,7 +929,7 @@
   <dimension ref="A1:U934"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -1008,7 +1018,7 @@
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="11">
         <v>36386</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1017,7 +1027,7 @@
       <c r="H2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J2" s="3" t="s">
@@ -1031,42 +1041,42 @@
       <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="12">
         <v>28605</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:16" ht="14.25" customHeight="1">
       <c r="A4" s="3" t="s">
@@ -1084,7 +1094,7 @@
       <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="11">
         <v>36290</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -1093,7 +1103,7 @@
       <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="3"/>
@@ -1107,44 +1117,44 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="12">
         <v>30081</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="P5" s="6"/>
+      <c r="J5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" ht="14.25" customHeight="1">
       <c r="A6" s="3" t="s">
@@ -1162,7 +1172,7 @@
       <c r="E6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="13">
         <v>28088</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -1171,7 +1181,7 @@
       <c r="H6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="J6" s="3"/>
@@ -1185,42 +1195,42 @@
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="12">
         <v>32966</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16" ht="14.25" customHeight="1">
       <c r="A8" s="3"/>
@@ -1236,7 +1246,7 @@
       <c r="E8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="11">
         <v>38541</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -1245,7 +1255,7 @@
       <c r="H8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="4" t="s">
         <v>49</v>
       </c>
       <c r="J8" s="3"/>
@@ -1259,44 +1269,44 @@
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="12">
         <v>31460</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="P9" s="6" t="s">
+      <c r="J9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1316,7 +1326,7 @@
       <c r="E10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="11">
         <v>28356</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -1325,7 +1335,7 @@
       <c r="H10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="4" t="s">
         <v>61</v>
       </c>
       <c r="J10" s="3"/>
@@ -1339,42 +1349,42 @@
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="12">
         <v>28601</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:16" ht="14.25" customHeight="1">
       <c r="A12" s="3" t="s">
@@ -1392,7 +1402,7 @@
       <c r="E12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="13">
         <v>31373</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -1401,7 +1411,7 @@
       <c r="H12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="4" t="s">
         <v>73</v>
       </c>
       <c r="J12" s="3"/>
@@ -1417,42 +1427,42 @@
       <c r="P12" s="3"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="12">
         <v>32673</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6" t="s">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1472,7 +1482,7 @@
       <c r="E14" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="11">
         <v>28648</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -1481,7 +1491,7 @@
       <c r="H14" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="4" t="s">
         <v>86</v>
       </c>
       <c r="J14" s="3"/>
@@ -1497,44 +1507,44 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="12">
         <v>35119</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:16" ht="14.25" customHeight="1">
       <c r="A16" s="3" t="s">
@@ -1552,7 +1562,7 @@
       <c r="E16" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="11">
         <v>27862</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -1561,7 +1571,7 @@
       <c r="H16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="4" t="s">
         <v>97</v>
       </c>
       <c r="J16" s="3"/>
@@ -1577,40 +1587,40 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="7">
+      <c r="E17" s="5"/>
+      <c r="F17" s="12">
         <v>28367</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="J17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
     </row>
     <row r="18" spans="1:16" ht="14.25" customHeight="1">
       <c r="A18" s="3" t="s">
@@ -1628,7 +1638,7 @@
       <c r="E18" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="11">
         <v>31483</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1637,7 +1647,7 @@
       <c r="H18" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="4" t="s">
         <v>109</v>
       </c>
       <c r="J18" s="3" t="s">
@@ -1651,40 +1661,40 @@
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="12">
         <v>33014</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
     </row>
     <row r="20" spans="1:16" ht="14.25" customHeight="1">
       <c r="A20" s="3" t="s">
@@ -1702,7 +1712,7 @@
       <c r="E20" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="11">
         <v>29359</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -1711,7 +1721,7 @@
       <c r="H20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="4" t="s">
         <v>119</v>
       </c>
       <c r="J20" s="3"/>
@@ -1725,44 +1735,44 @@
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="12">
         <v>38232</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="P21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P21" s="5"/>
     </row>
     <row r="22" spans="1:16" ht="14.25" customHeight="1">
       <c r="A22" s="3" t="s">
@@ -1780,7 +1790,7 @@
       <c r="E22" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="11">
         <v>30086</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -1789,7 +1799,7 @@
       <c r="H22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="I22" s="4" t="s">
         <v>131</v>
       </c>
       <c r="J22" s="3"/>
@@ -1801,40 +1811,40 @@
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="12">
         <v>28495</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I23" s="9" t="s">
+      <c r="I23" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6" t="s">
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1854,7 +1864,7 @@
       <c r="E24" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="11">
         <v>34567</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -1863,7 +1873,7 @@
       <c r="H24" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="4" t="s">
         <v>142</v>
       </c>
       <c r="J24" s="3" t="s">
@@ -1879,40 +1889,40 @@
       <c r="P24" s="3"/>
     </row>
     <row r="25" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="12">
         <v>38500</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G25" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="9" t="s">
+      <c r="H25" s="5"/>
+      <c r="I25" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6" t="s">
+      <c r="J25" s="5"/>
+      <c r="K25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1932,7 +1942,7 @@
       <c r="E26" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="11">
         <v>36329</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -1941,7 +1951,7 @@
       <c r="H26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="4" t="s">
         <v>154</v>
       </c>
       <c r="J26" s="3"/>
@@ -1957,44 +1967,44 @@
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="1:16" ht="14.25" customHeight="1">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="12">
         <v>29787</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H27" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I27" s="9" t="s">
+      <c r="I27" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
     </row>
     <row r="28" spans="1:16" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:16" ht="14.25" customHeight="1"/>
@@ -2002,488 +2012,488 @@
     <row r="31" spans="1:16" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:16" ht="14.25" customHeight="1"/>
     <row r="33" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="U33" s="8"/>
     </row>
     <row r="34" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
-      <c r="T34" s="11"/>
-      <c r="U34" s="11"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
     </row>
     <row r="35" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="11"/>
-      <c r="U35" s="11"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="8"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="8"/>
+      <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="U35" s="8"/>
     </row>
     <row r="36" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
     </row>
     <row r="37" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="11"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
     </row>
     <row r="38" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="11"/>
-      <c r="T38" s="11"/>
-      <c r="U38" s="11"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="U38" s="8"/>
     </row>
     <row r="39" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-      <c r="T39" s="11"/>
-      <c r="U39" s="11"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="8"/>
+      <c r="T39" s="8"/>
+      <c r="U39" s="8"/>
     </row>
     <row r="40" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="11"/>
-      <c r="T40" s="11"/>
-      <c r="U40" s="11"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="8"/>
+      <c r="T40" s="8"/>
+      <c r="U40" s="8"/>
     </row>
     <row r="41" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="11"/>
-      <c r="U41" s="11"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
     </row>
     <row r="42" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="12"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-      <c r="T42" s="11"/>
-      <c r="U42" s="11"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
     </row>
     <row r="43" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="12"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
-      <c r="S43" s="11"/>
-      <c r="T43" s="11"/>
-      <c r="U43" s="11"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
     </row>
     <row r="44" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="11"/>
-      <c r="S44" s="11"/>
-      <c r="T44" s="11"/>
-      <c r="U44" s="11"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
     </row>
     <row r="45" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="11"/>
-      <c r="S45" s="11"/>
-      <c r="T45" s="11"/>
-      <c r="U45" s="11"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
     </row>
     <row r="46" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="12"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="11"/>
-      <c r="S46" s="11"/>
-      <c r="T46" s="11"/>
-      <c r="U46" s="11"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="8"/>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
+      <c r="O46" s="8"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
     </row>
     <row r="47" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="12"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
-      <c r="T47" s="11"/>
-      <c r="U47" s="11"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="8"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="8"/>
+      <c r="R47" s="8"/>
+      <c r="S47" s="8"/>
+      <c r="T47" s="8"/>
+      <c r="U47" s="8"/>
     </row>
     <row r="48" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="11"/>
-      <c r="S48" s="11"/>
-      <c r="T48" s="11"/>
-      <c r="U48" s="11"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="8"/>
+      <c r="M48" s="8"/>
+      <c r="N48" s="8"/>
+      <c r="O48" s="8"/>
+      <c r="P48" s="8"/>
+      <c r="Q48" s="8"/>
+      <c r="R48" s="8"/>
+      <c r="S48" s="8"/>
+      <c r="T48" s="8"/>
+      <c r="U48" s="8"/>
     </row>
     <row r="49" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="12"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="11"/>
-      <c r="R49" s="11"/>
-      <c r="S49" s="11"/>
-      <c r="T49" s="11"/>
-      <c r="U49" s="11"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="8"/>
+      <c r="R49" s="8"/>
+      <c r="S49" s="8"/>
+      <c r="T49" s="8"/>
+      <c r="U49" s="8"/>
     </row>
     <row r="50" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11"/>
-      <c r="N50" s="11"/>
-      <c r="O50" s="11"/>
-      <c r="P50" s="11"/>
-      <c r="Q50" s="11"/>
-      <c r="R50" s="11"/>
-      <c r="S50" s="11"/>
-      <c r="T50" s="11"/>
-      <c r="U50" s="11"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="8"/>
+      <c r="M50" s="8"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="8"/>
+      <c r="P50" s="8"/>
+      <c r="Q50" s="8"/>
+      <c r="R50" s="8"/>
+      <c r="S50" s="8"/>
+      <c r="T50" s="8"/>
+      <c r="U50" s="8"/>
     </row>
     <row r="51" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="11"/>
-      <c r="S51" s="11"/>
-      <c r="T51" s="11"/>
-      <c r="U51" s="11"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="8"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
+      <c r="R51" s="8"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
     </row>
     <row r="52" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="11"/>
-      <c r="S52" s="11"/>
-      <c r="T52" s="11"/>
-      <c r="U52" s="11"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="8"/>
+      <c r="M52" s="8"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="8"/>
+      <c r="P52" s="8"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
     </row>
     <row r="53" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="11"/>
-      <c r="S53" s="11"/>
-      <c r="T53" s="11"/>
-      <c r="U53" s="11"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="8"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="8"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="8"/>
+      <c r="T53" s="8"/>
+      <c r="U53" s="8"/>
     </row>
     <row r="54" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="11"/>
-      <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
-      <c r="O54" s="11"/>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="11"/>
-      <c r="S54" s="11"/>
-      <c r="T54" s="11"/>
-      <c r="U54" s="11"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="8"/>
+      <c r="M54" s="8"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="8"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="8"/>
+      <c r="U54" s="8"/>
     </row>
     <row r="55" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="11"/>
-      <c r="S55" s="11"/>
-      <c r="T55" s="11"/>
-      <c r="U55" s="11"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="8"/>
+      <c r="R55" s="8"/>
+      <c r="S55" s="8"/>
+      <c r="T55" s="8"/>
+      <c r="U55" s="8"/>
     </row>
     <row r="56" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-      <c r="S56" s="11"/>
-      <c r="T56" s="11"/>
-      <c r="U56" s="11"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="8"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="8"/>
+      <c r="R56" s="8"/>
+      <c r="S56" s="8"/>
+      <c r="T56" s="8"/>
+      <c r="U56" s="8"/>
     </row>
     <row r="57" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="11"/>
-      <c r="S57" s="11"/>
-      <c r="T57" s="11"/>
-      <c r="U57" s="11"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="8"/>
+      <c r="R57" s="8"/>
+      <c r="S57" s="8"/>
+      <c r="T57" s="8"/>
+      <c r="U57" s="8"/>
     </row>
     <row r="58" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="12"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="11"/>
-      <c r="S58" s="11"/>
-      <c r="T58" s="11"/>
-      <c r="U58" s="11"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="8"/>
+      <c r="Q58" s="8"/>
+      <c r="R58" s="8"/>
+      <c r="S58" s="8"/>
+      <c r="T58" s="8"/>
+      <c r="U58" s="8"/>
     </row>
     <row r="59" spans="6:21" ht="14.25" customHeight="1">
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="12"/>
-      <c r="L59" s="11"/>
-      <c r="M59" s="11"/>
-      <c r="N59" s="11"/>
-      <c r="O59" s="11"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="11"/>
-      <c r="S59" s="11"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8"/>
+      <c r="N59" s="8"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="8"/>
+      <c r="Q59" s="8"/>
+      <c r="R59" s="8"/>
+      <c r="S59" s="8"/>
     </row>
     <row r="60" spans="6:21" ht="14.25" customHeight="1"/>
     <row r="61" spans="6:21" ht="14.25" customHeight="1"/>

</xml_diff>